<commit_message>
feat: update template files
</commit_message>
<xml_diff>
--- a/public/files/保安员工导入模板.xlsx
+++ b/public/files/保安员工导入模板.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>保安员工导入模板</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">注意事项
 </t>
     </r>
@@ -53,6 +59,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
       <t>所在学校</t>
     </r>
     <r>
@@ -94,6 +107,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>籍贯</t>
     </r>
     <r>
@@ -129,6 +149,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>出生日期</t>
     </r>
     <r>
@@ -164,6 +191,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
       <t>住址</t>
     </r>
     <r>
@@ -198,43 +232,40 @@
     </r>
   </si>
   <si>
-    <t>张三</t>
+    <t>黄春华</t>
   </si>
   <si>
     <t>男</t>
   </si>
   <si>
-    <t>34222419980402900</t>
-  </si>
-  <si>
-    <t>17775488765</t>
-  </si>
-  <si>
-    <t>10200932</t>
-  </si>
-  <si>
-    <t>张家港保安有限公司</t>
-  </si>
-  <si>
-    <t>zhigonghao131</t>
-  </si>
-  <si>
-    <t>满族</t>
-  </si>
-  <si>
-    <t>江苏宿迁</t>
-  </si>
-  <si>
-    <t>1965-5-5</t>
-  </si>
-  <si>
-    <t>江苏张家港市</t>
+    <t>320582197103016717</t>
+  </si>
+  <si>
+    <t>13915692786</t>
+  </si>
+  <si>
+    <t>32052016006687</t>
+  </si>
+  <si>
+    <t>张家港市保安服务有限公司</t>
+  </si>
+  <si>
+    <t>白鹿小学</t>
+  </si>
+  <si>
+    <t>汉族</t>
+  </si>
+  <si>
+    <t>1971-03-01</t>
+  </si>
+  <si>
+    <t>江苏省张家港市常阴沙管理区常东社区四组39号</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -954,7 +985,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -990,9 +1021,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1348,8 +1376,8 @@
   <sheetPr/>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3"/>
@@ -1357,10 +1385,11 @@
     <col min="1" max="1" width="15.3846153846154" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.49038461538461" style="2" customWidth="1"/>
     <col min="3" max="5" width="19.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.875" style="2" customWidth="1"/>
-    <col min="7" max="10" width="19.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.6923076923077" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.1538461538462" style="2" customWidth="1"/>
+    <col min="8" max="10" width="19.25" style="2" customWidth="1"/>
     <col min="11" max="11" width="25.3173076923077" style="2" customWidth="1"/>
-    <col min="12" max="12" width="33.9711538461538" style="2" customWidth="1"/>
+    <col min="12" max="12" width="57.1538461538462" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1392,9 +1421,9 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" ht="17" spans="1:12">
       <c r="A3" s="7" t="s">
@@ -1424,10 +1453,10 @@
       <c r="I3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -1453,21 +1482,19 @@
       <c r="F4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="11"/>
+      <c r="K4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add employee address input
</commit_message>
<xml_diff>
--- a/public/files/保安员工导入模板.xlsx
+++ b/public/files/保安员工导入模板.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>保安员工导入模板</t>
   </si>
@@ -232,34 +232,103 @@
     </r>
   </si>
   <si>
+    <t>缪凯鑫</t>
+  </si>
+  <si>
+    <t>320582199405150515</t>
+  </si>
+  <si>
+    <t>32052023001585</t>
+  </si>
+  <si>
+    <t>张家港市保安服务有限公司</t>
+  </si>
+  <si>
+    <t>白鹿小学</t>
+  </si>
+  <si>
     <t>黄春华</t>
   </si>
   <si>
-    <t>男</t>
-  </si>
-  <si>
     <t>320582197103016717</t>
   </si>
   <si>
-    <t>13915692786</t>
-  </si>
-  <si>
     <t>32052016006687</t>
   </si>
   <si>
-    <t>张家港市保安服务有限公司</t>
-  </si>
-  <si>
-    <t>白鹿小学</t>
-  </si>
-  <si>
-    <t>汉族</t>
-  </si>
-  <si>
-    <t>1971-03-01</t>
-  </si>
-  <si>
-    <t>江苏省张家港市常阴沙管理区常东社区四组39号</t>
+    <t>席缪锋</t>
+  </si>
+  <si>
+    <t>320582197712029118</t>
+  </si>
+  <si>
+    <t>32052018010855</t>
+  </si>
+  <si>
+    <t>夏建东</t>
+  </si>
+  <si>
+    <t>320582196807020517</t>
+  </si>
+  <si>
+    <t>32052013004654</t>
+  </si>
+  <si>
+    <t>许枝平</t>
+  </si>
+  <si>
+    <t>320521197101130513</t>
+  </si>
+  <si>
+    <t>32052017009778</t>
+  </si>
+  <si>
+    <t>尹广之</t>
+  </si>
+  <si>
+    <t>320521197904185112</t>
+  </si>
+  <si>
+    <t>32052022001775</t>
+  </si>
+  <si>
+    <t>张建华</t>
+  </si>
+  <si>
+    <t>321024197401090413</t>
+  </si>
+  <si>
+    <t>32052016009357</t>
+  </si>
+  <si>
+    <t>丁苏春</t>
+  </si>
+  <si>
+    <t>320582198104014814</t>
+  </si>
+  <si>
+    <t>32052017007625</t>
+  </si>
+  <si>
+    <t>白鹿幼儿园</t>
+  </si>
+  <si>
+    <t>沈志文</t>
+  </si>
+  <si>
+    <t>320521196802080518</t>
+  </si>
+  <si>
+    <t>32052018010887</t>
+  </si>
+  <si>
+    <t>张小泉</t>
+  </si>
+  <si>
+    <t>320521196903052655</t>
+  </si>
+  <si>
+    <t>32052012024856</t>
   </si>
 </sst>
 </file>
@@ -985,44 +1054,65 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1374,127 +1464,348 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="15.3846153846154" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.49038461538461" style="2" customWidth="1"/>
-    <col min="3" max="5" width="19.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.6923076923077" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.1538461538462" style="2" customWidth="1"/>
-    <col min="8" max="10" width="19.25" style="2" customWidth="1"/>
+    <col min="3" max="5" width="19.25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.6923076923077" style="3" customWidth="1"/>
+    <col min="7" max="7" width="32.1538461538462" style="3" customWidth="1"/>
+    <col min="8" max="10" width="19.25" style="3" customWidth="1"/>
     <col min="11" max="11" width="25.3173076923077" style="2" customWidth="1"/>
-    <col min="12" max="12" width="57.1538461538462" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="2"/>
+    <col min="12" max="12" width="57.1538461538462" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:12">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" ht="60" customHeight="1" spans="1:12">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" ht="17" spans="1:12">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="2" t="str">
+        <f>IF(MOD(MID(C4,17,1),2)=0,"女","男")</f>
+        <v>男</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="F4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="G4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="18" t="str">
+        <f>CONCATENATE(MID(C4,7,4),"-",MID(C4,11,2),"-",MID(C4,13,2))</f>
+        <v>1994-05-15</v>
+      </c>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="B5" s="2" t="str">
+        <f>IF(MOD(MID(C5,17,1),2)=0,"女","男")</f>
+        <v>男</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11" t="s">
+      <c r="F5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="18" t="str">
+        <f t="shared" ref="K5:K13" si="0">CONCATENATE(MID(C5,7,4),"-",MID(C5,11,2),"-",MID(C5,13,2))</f>
+        <v>1971-03-01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="B6" s="2" t="str">
+        <f>IF(MOD(MID(C6,17,1),2)=0,"女","男")</f>
+        <v>男</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1977-12-02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f t="shared" ref="B6:B13" si="1">IF(MOD(MID(C7,17,1),2)=0,"女","男")</f>
+        <v>男</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1968-07-02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>男</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1971-01-13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>男</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1979-04-18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>男</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1974-01-09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>男</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1981-04-01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>男</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1968-02-08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>男</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1969-03-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>